<commit_message>
Fix control size and color 2
</commit_message>
<xml_diff>
--- a/public/dist/excel/templateBulkImport.xlsx
+++ b/public/dist/excel/templateBulkImport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64-2\www\mbc-middleware\public\dist\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E389C75-C8B6-4C03-8CEA-A5606FCFEF72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8150656F-FF48-4339-8115-9A0E2DD8197E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26220" yWindow="960" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="27">
   <si>
     <t>title</t>
   </si>
@@ -107,7 +107,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,8 +249,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -428,6 +435,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -606,9 +619,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -969,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AA1" activeCellId="1" sqref="Z1 AA1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,22 +1009,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1019,19 +1036,19 @@
       <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="O1" s="1" t="s">

</xml_diff>